<commit_message>
Adding more detail to project description
</commit_message>
<xml_diff>
--- a/Fall 2025/White Box Models/Model Tournament/Tournament Bracket.xlsx
+++ b/Fall 2025/White Box Models/Model Tournament/Tournament Bracket.xlsx
@@ -1107,7 +1107,7 @@
       <c r="L16" s="29" t="n"/>
       <c r="M16" s="30" t="inlineStr">
         <is>
-          <t>Logistic Regression #1</t>
+          <t>SVM #1</t>
         </is>
       </c>
       <c r="N16" s="29" t="n"/>
@@ -1292,7 +1292,7 @@
       <c r="P24" s="40" t="n"/>
       <c r="Q24" s="56" t="inlineStr">
         <is>
-          <t>Logistic Regression #1</t>
+          <t>SVM #1</t>
         </is>
       </c>
       <c r="R24" s="41" t="n"/>
@@ -1493,7 +1493,7 @@
       <c r="L32" s="29" t="n"/>
       <c r="M32" s="30" t="inlineStr">
         <is>
-          <t>Gradient Boost #1</t>
+          <t>Gradient Boost #2</t>
         </is>
       </c>
       <c r="N32" s="29" t="n"/>
@@ -1539,7 +1539,7 @@
       <c r="E34" s="13" t="n"/>
       <c r="F34" s="49" t="inlineStr">
         <is>
-          <t>Gradient Boost #1</t>
+          <t>Gradient Boost #2</t>
         </is>
       </c>
       <c r="G34" s="14" t="n"/>
@@ -1592,7 +1592,7 @@
       <c r="H36" s="22" t="n"/>
       <c r="I36" s="55" t="inlineStr">
         <is>
-          <t>Gradient Boost #1</t>
+          <t>Gradient Boost #2</t>
         </is>
       </c>
       <c r="J36" s="22" t="n"/>

</xml_diff>